<commit_message>
Uploaded the files of the five last days
</commit_message>
<xml_diff>
--- a/files/Matières/Emplois du temps/T/week-end du 21 au 22 11 2020.xlsx
+++ b/files/Matières/Emplois du temps/T/week-end du 21 au 22 11 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry PC\Documents\001 Github prog Sharing\Backup-of-matiere\files\Matières\Emplois du temps\T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2791309C-998C-4843-8C03-2AA5E9190956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC885E2A-549E-451E-AA7A-5D33307A2C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,12 +932,12 @@
       <c r="C11" s="3">
         <v>0.40625</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="4"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -947,10 +947,10 @@
       <c r="C12" s="3">
         <v>0.41666666666666702</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -960,10 +960,10 @@
       <c r="C13" s="3">
         <v>0.42708333333333298</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -973,10 +973,10 @@
       <c r="C14" s="3">
         <v>0.4375</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -986,10 +986,10 @@
       <c r="C15" s="3">
         <v>0.44791666666666702</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>

</xml_diff>